<commit_message>
Atualização automática de VERA_CRUZ.xlsx
</commit_message>
<xml_diff>
--- a/VERA_CRUZ.xlsx
+++ b/VERA_CRUZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4AAE109-9B6B-438A-B18C-8597A8CECA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EB00E7F-F5C8-4EAE-B7DE-6779487907AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1194,7 +1194,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{33166C19-C45D-4CCC-B478-0D30A7482AB4}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F3B17A06-B1B9-4A06-AEBC-BAE4C5A9FE74}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1224,10 +1224,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{706EF7F0-51CC-434A-AC01-E7A69A308785}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6D6F32-815E-46A2-9F91-6AFA3909EDDD}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1265,7 +1265,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21CB5D85-D547-4171-824E-B5E8628E9786}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44ECB04F-C97E-4F2C-80BC-BD0D828BD8B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1328,7 +1328,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2E0DDB9-BE1B-479F-B06A-78543F1FFB06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24FD08DD-524F-4856-9C2F-186F2D81555A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1347,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{913BAA1C-14CC-A1BE-89B5-36171663B27D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BE8A4B0-14DB-8520-0EF4-ACD517F599EA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1396,7 +1396,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B481166D-EDAD-2FE3-639F-C1DCEA7E161F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AECD06FB-3CCD-F988-2304-EC147DE34674}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1415,7 +1415,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21EC832F-78E8-BD02-BB1F-CD81AF42FF98}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A69CE17C-C96A-7876-170B-8055EA8E8A50}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1446,7 +1446,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAB4791D-A8E3-921F-1712-FA697A7FDFFF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C51A7AD-5027-2700-0A5E-8924AC2A903E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1477,7 +1477,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE17E349-222B-7FFA-B4B2-180047E4731E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB0096A-B881-A122-02F8-07F0ADBEE493}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1520,7 +1520,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4F55782-4CEE-4146-9BD8-FD53C22CF4B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C68236F-A6A9-49DE-9B32-C911E999AD04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1558,7 +1558,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5709CF3B-607D-4555-8121-093D3C6B0C2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1621EC-28C3-4B85-B53B-52A1DCDAA8E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1601,7 +1601,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A68294AC-691B-4F7C-B6CD-796F5AD8C3F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2E786E-370B-4F38-9B73-701DB8E50418}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1914,7 +1914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C95D41-7B1D-423E-BE01-7574713F052B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB040B79-BFD3-4F7A-BA4D-D365CDC31544}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>